<commit_message>
Adding Lab 6 HumMod data. Several issues are present.
</commit_message>
<xml_diff>
--- a/06_water_load/water_load_data.xlsx
+++ b/06_water_load/water_load_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="23">
   <si>
     <t>Time</t>
   </si>
@@ -73,13 +73,25 @@
   </si>
   <si>
     <t>mL/min</t>
+  </si>
+  <si>
+    <t>QCP</t>
+  </si>
+  <si>
+    <t>HumMod</t>
+  </si>
+  <si>
+    <t>The water load is readily available and easy to use, but it does not appear to have any actual effect on the simulation. The numbers remained exactly the same.</t>
+  </si>
+  <si>
+    <t>There is no ADH Clamp in HumMod, but since the ADH concentration is not changing anyway, the clamp is not necessary to complete the lab for a clamped ADH value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,13 +105,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -129,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -141,6 +165,15 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,15 +468,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
+      <selection activeCell="U29" sqref="U29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -468,8 +501,38 @@
       <c r="H1" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="3">
+        <v>0</v>
+      </c>
+      <c r="N1" s="3">
+        <v>1</v>
+      </c>
+      <c r="O1" s="3">
+        <v>2</v>
+      </c>
+      <c r="P1" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="3">
+        <v>6</v>
+      </c>
+      <c r="R1" s="3">
+        <v>1</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="T1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="15.75" thickBot="1">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -490,8 +553,28 @@
         <v>4</v>
       </c>
       <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" ht="30.75" thickBot="1">
+      <c r="L2" s="2"/>
+      <c r="M2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" s="4"/>
+    </row>
+    <row r="3" spans="1:20" ht="30.75" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -516,8 +599,32 @@
       <c r="H3" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="30.75" thickBot="1">
+      <c r="L3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="2">
+        <v>949.4</v>
+      </c>
+      <c r="N3" s="2">
+        <v>949.4</v>
+      </c>
+      <c r="O3" s="2">
+        <v>949.4</v>
+      </c>
+      <c r="P3" s="2">
+        <v>949.4</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>949.4</v>
+      </c>
+      <c r="R3" s="2">
+        <v>949.4</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="30.75" thickBot="1">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -542,8 +649,32 @@
       <c r="H4" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="30.75" thickBot="1">
+      <c r="L4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="2">
+        <v>3081</v>
+      </c>
+      <c r="N4" s="2">
+        <v>3081</v>
+      </c>
+      <c r="O4" s="2">
+        <v>3081</v>
+      </c>
+      <c r="P4" s="2">
+        <v>3081</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>3081</v>
+      </c>
+      <c r="R4" s="2">
+        <v>3081</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="30.75" thickBot="1">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -568,8 +699,32 @@
       <c r="H5" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1">
+      <c r="L5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="2">
+        <v>275.7</v>
+      </c>
+      <c r="N5" s="2">
+        <v>275.7</v>
+      </c>
+      <c r="O5" s="2">
+        <v>275.7</v>
+      </c>
+      <c r="P5" s="2">
+        <v>275.7</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>275.7</v>
+      </c>
+      <c r="R5" s="2">
+        <v>275.7</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="15.75" thickBot="1">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -594,8 +749,32 @@
       <c r="H6" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="30.75" thickBot="1">
+      <c r="L6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="N6" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="O6" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="P6" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="R6" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="30.75" thickBot="1">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -620,8 +799,32 @@
       <c r="H7" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="30.75" thickBot="1">
+      <c r="L7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="N7" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="O7" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="P7" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="R7" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="30.75" thickBot="1">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -646,8 +849,32 @@
       <c r="H8" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="30.75" thickBot="1">
+      <c r="L8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="R8" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="30.75" thickBot="1">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -672,13 +899,40 @@
       <c r="H9" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="45.75" thickBot="1">
+      <c r="L9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="2">
+        <v>687.3</v>
+      </c>
+      <c r="N9" s="2">
+        <v>687.3</v>
+      </c>
+      <c r="O9" s="2">
+        <v>687.3</v>
+      </c>
+      <c r="P9" s="2">
+        <v>687.3</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>687.3</v>
+      </c>
+      <c r="R9" s="2">
+        <v>687.3</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="45.75" thickBot="1">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1">
+      <c r="L11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="15.75" thickBot="1">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -703,8 +957,38 @@
       <c r="H12" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1">
+      <c r="I12" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0</v>
+      </c>
+      <c r="N12" s="3">
+        <v>1</v>
+      </c>
+      <c r="O12" s="3">
+        <v>2</v>
+      </c>
+      <c r="P12" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>6</v>
+      </c>
+      <c r="R12" s="3">
+        <v>1</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="T12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="15.75" thickBot="1">
       <c r="A13" s="2"/>
       <c r="B13" s="3" t="s">
         <v>1</v>
@@ -725,8 +1009,28 @@
         <v>4</v>
       </c>
       <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" ht="30.75" thickBot="1">
+      <c r="L13" s="2"/>
+      <c r="M13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S13" s="4"/>
+    </row>
+    <row r="14" spans="1:20" ht="30.75" thickBot="1">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -751,8 +1055,32 @@
       <c r="H14" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="30.75" thickBot="1">
+      <c r="L14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M14" s="2">
+        <v>949.4</v>
+      </c>
+      <c r="N14" s="2">
+        <v>949.4</v>
+      </c>
+      <c r="O14" s="2">
+        <v>949.4</v>
+      </c>
+      <c r="P14" s="2">
+        <v>949.4</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>949.4</v>
+      </c>
+      <c r="R14" s="2">
+        <v>949.4</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="30.75" thickBot="1">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -777,8 +1105,32 @@
       <c r="H15" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="30.75" thickBot="1">
+      <c r="L15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M15" s="2">
+        <v>3081</v>
+      </c>
+      <c r="N15" s="2">
+        <v>3081</v>
+      </c>
+      <c r="O15" s="2">
+        <v>3081</v>
+      </c>
+      <c r="P15" s="2">
+        <v>3081</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>3081</v>
+      </c>
+      <c r="R15" s="2">
+        <v>3081</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="30.75" thickBot="1">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
@@ -803,8 +1155,32 @@
       <c r="H16" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1">
+      <c r="L16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M16" s="2">
+        <v>275.7</v>
+      </c>
+      <c r="N16" s="2">
+        <v>275.7</v>
+      </c>
+      <c r="O16" s="2">
+        <v>275.7</v>
+      </c>
+      <c r="P16" s="2">
+        <v>275.7</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>275.7</v>
+      </c>
+      <c r="R16" s="2">
+        <v>275.7</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="15.75" thickBot="1">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -829,8 +1205,32 @@
       <c r="H17" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="30.75" thickBot="1">
+      <c r="L17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M17" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="N17" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="O17" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="P17" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="R17" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="S17" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="30.75" thickBot="1">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -855,8 +1255,32 @@
       <c r="H18" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="30.75" thickBot="1">
+      <c r="L18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="N18" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="O18" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="P18" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="R18" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="30.75" thickBot="1">
       <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
@@ -881,8 +1305,32 @@
       <c r="H19" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="30.75" thickBot="1">
+      <c r="L19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="N19" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="O19" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="P19" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="R19" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="S19" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="30.75" thickBot="1">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
@@ -907,8 +1355,80 @@
       <c r="H20" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="L20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M20" s="2">
+        <v>687.3</v>
+      </c>
+      <c r="N20" s="2">
+        <v>687.3</v>
+      </c>
+      <c r="O20" s="2">
+        <v>687.3</v>
+      </c>
+      <c r="P20" s="2">
+        <v>687.3</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>687.3</v>
+      </c>
+      <c r="R20" s="2">
+        <v>687.3</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="L22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="L25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="L22:S23"/>
+    <mergeCell ref="L25:S26"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixing Lab 6 charts
</commit_message>
<xml_diff>
--- a/06_water_load/water_load_data.xlsx
+++ b/06_water_load/water_load_data.xlsx
@@ -170,7 +170,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -191,34 +191,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -237,41 +217,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -574,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AG26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U10" workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13:AF19"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AL16" sqref="AL16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -659,7 +604,7 @@
       <c r="AF1" s="3">
         <v>1</v>
       </c>
-      <c r="AG1" s="4"/>
+      <c r="AG1" s="9"/>
     </row>
     <row r="2" spans="1:33" ht="15.75" thickBot="1">
       <c r="A2" s="2"/>
@@ -724,7 +669,7 @@
       <c r="AF2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AG2" s="4"/>
+      <c r="AG2" s="9"/>
     </row>
     <row r="3" spans="1:33" ht="30.75" thickBot="1">
       <c r="A3" s="2" t="s">
@@ -1297,7 +1242,7 @@
       <c r="AF11" s="3">
         <v>1</v>
       </c>
-      <c r="AG11" s="4"/>
+      <c r="AG11" s="9"/>
     </row>
     <row r="12" spans="1:33" ht="15.75" thickBot="1">
       <c r="A12" s="2" t="s">
@@ -1373,7 +1318,7 @@
       <c r="AF12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AG12" s="4"/>
+      <c r="AG12" s="9"/>
     </row>
     <row r="13" spans="1:33" ht="30.75" thickBot="1">
       <c r="A13" s="2"/>
@@ -1443,6 +1388,7 @@
         <f t="shared" si="7"/>
         <v>0.78123827392120071</v>
       </c>
+      <c r="AG13" s="9"/>
     </row>
     <row r="14" spans="1:33" ht="30.75" thickBot="1">
       <c r="A14" s="2" t="s">
@@ -1520,6 +1466,7 @@
         <f t="shared" ref="AF14:AF19" si="13">ABS((G15-R15)/G15)</f>
         <v>3.4586971121558091E-2</v>
       </c>
+      <c r="AG14" s="9"/>
     </row>
     <row r="15" spans="1:33" ht="30.75" thickBot="1">
       <c r="A15" s="2" t="s">
@@ -1597,6 +1544,7 @@
         <f t="shared" si="13"/>
         <v>3.6013986013986053E-2</v>
       </c>
+      <c r="AG15" s="9"/>
     </row>
     <row r="16" spans="1:33" ht="30.75" thickBot="1">
       <c r="A16" s="2" t="s">
@@ -1674,8 +1622,9 @@
         <f t="shared" si="13"/>
         <v>0.16161616161616157</v>
       </c>
-    </row>
-    <row r="17" spans="1:32" ht="30.75" thickBot="1">
+      <c r="AG16" s="9"/>
+    </row>
+    <row r="17" spans="1:33" ht="30.75" thickBot="1">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -1751,8 +1700,9 @@
         <f t="shared" si="13"/>
         <v>0.13913043478260864</v>
       </c>
-    </row>
-    <row r="18" spans="1:32" ht="30.75" thickBot="1">
+      <c r="AG17" s="9"/>
+    </row>
+    <row r="18" spans="1:33" ht="30.75" thickBot="1">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -1828,8 +1778,9 @@
         <f t="shared" si="13"/>
         <v>0.40625</v>
       </c>
-    </row>
-    <row r="19" spans="1:32" ht="30.75" thickBot="1">
+      <c r="AG18" s="9"/>
+    </row>
+    <row r="19" spans="1:33" ht="30.75" thickBot="1">
       <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
@@ -1905,8 +1856,9 @@
         <f t="shared" si="13"/>
         <v>0.40596369922212622</v>
       </c>
-    </row>
-    <row r="20" spans="1:32" ht="30.75" thickBot="1">
+      <c r="AG19" s="9"/>
+    </row>
+    <row r="20" spans="1:33" ht="30.75" thickBot="1">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
@@ -1956,7 +1908,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:32">
+    <row r="22" spans="1:33">
       <c r="L22" s="5" t="s">
         <v>21</v>
       </c>
@@ -1968,7 +1920,7 @@
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
     </row>
-    <row r="23" spans="1:32">
+    <row r="23" spans="1:33">
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
@@ -1978,7 +1930,7 @@
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
     </row>
-    <row r="25" spans="1:32">
+    <row r="25" spans="1:33">
       <c r="L25" s="7" t="s">
         <v>22</v>
       </c>
@@ -1990,7 +1942,7 @@
       <c r="R25" s="7"/>
       <c r="S25" s="7"/>
     </row>
-    <row r="26" spans="1:32">
+    <row r="26" spans="1:33">
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
@@ -2006,20 +1958,20 @@
     <mergeCell ref="L25:S26"/>
   </mergeCells>
   <conditionalFormatting sqref="AA3:AF9">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
       <formula>0.5</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA13:AF19">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>0.5</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>